<commit_message>
Move NDVI predictions from manager script to Spectral component
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/Dookie2024/DookieEVA2024.xlsx
+++ b/Tests/Validation/Wheat/Dookie2024/DookieEVA2024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\ApsimX\Tests\Validation\Wheat\Dookie2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\Dookie2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D9982C-FD66-4D8F-8F85-4E7B512A0CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8A86FD-74FC-4985-AAED-BA846737B15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="-11640" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,9 +38,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="34">
-  <si>
-    <t>NDVIModel.Script.NDVI</t>
-  </si>
   <si>
     <t>Wheat.Phenology.HaunStage</t>
   </si>
@@ -140,6 +137,9 @@
   <si>
     <t>ParameterName</t>
   </si>
+  <si>
+    <t>Spectral.NDVI</t>
+  </si>
 </sst>
 </file>
 
@@ -147,7 +147,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -219,8 +219,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -233,15 +233,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="167" formatCode="dd\-mmm\-yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="dd\-mmm\-yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="dd\-mmm\-yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4694,7 +4688,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4FFA427B-6337-4DA0-868A-A49EE0DF7D9D}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4FFA427B-6337-4DA0-868A-A49EE0DF7D9D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F10:I19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField axis="axisRow" showAll="0">
@@ -4783,7 +4777,7 @@
     <dataField name="Max of Clock.Today" fld="1" subtotal="max" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="8">
@@ -5101,71 +5095,71 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>45443</v>
@@ -5174,9 +5168,9 @@
         <v>0.29249999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
         <v>45460</v>
@@ -5185,9 +5179,9 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
         <v>45474</v>
@@ -5196,9 +5190,9 @@
         <v>0.52249999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>45487</v>
@@ -5207,9 +5201,9 @@
         <v>0.60250000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2">
         <v>45502</v>
@@ -5218,9 +5212,9 @@
         <v>0.65249999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>45513</v>
@@ -5229,9 +5223,9 @@
         <v>0.69499999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>45526</v>
@@ -5240,9 +5234,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>45548</v>
@@ -5251,9 +5245,9 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
         <v>45559</v>
@@ -5262,9 +5256,9 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>45571</v>
@@ -5273,9 +5267,9 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
         <v>45582</v>
@@ -5284,9 +5278,9 @@
         <v>0.59749999999999992</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
         <v>45594</v>
@@ -5295,9 +5289,9 @@
         <v>0.4975</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2">
         <v>45609</v>
@@ -5306,9 +5300,9 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
         <v>45443</v>
@@ -5317,9 +5311,9 @@
         <v>0.30249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>45460</v>
@@ -5328,9 +5322,9 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>45474</v>
@@ -5339,9 +5333,9 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>45487</v>
@@ -5350,9 +5344,9 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2">
         <v>45502</v>
@@ -5361,9 +5355,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2">
         <v>45513</v>
@@ -5372,9 +5366,9 @@
         <v>0.68500000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="2">
         <v>45526</v>
@@ -5383,9 +5377,9 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2">
         <v>45548</v>
@@ -5394,9 +5388,9 @@
         <v>0.84250000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="2">
         <v>45559</v>
@@ -5405,9 +5399,9 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="2">
         <v>45571</v>
@@ -5416,9 +5410,9 @@
         <v>0.73750000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="2">
         <v>45582</v>
@@ -5427,9 +5421,9 @@
         <v>0.57750000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2">
         <v>45594</v>
@@ -5438,9 +5432,9 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2">
         <v>45609</v>
@@ -5449,9 +5443,9 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="2">
         <v>45443</v>
@@ -5460,9 +5454,9 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="2">
         <v>45460</v>
@@ -5471,9 +5465,9 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="2">
         <v>45474</v>
@@ -5482,9 +5476,9 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="2">
         <v>45487</v>
@@ -5493,9 +5487,9 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B32" s="2">
         <v>45502</v>
@@ -5504,9 +5498,9 @@
         <v>0.57250000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33" s="2">
         <v>45513</v>
@@ -5515,9 +5509,9 @@
         <v>0.60250000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="2">
         <v>45526</v>
@@ -5526,9 +5520,9 @@
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2">
         <v>45548</v>
@@ -5537,9 +5531,9 @@
         <v>0.80249999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="2">
         <v>45559</v>
@@ -5548,9 +5542,9 @@
         <v>0.75249999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37" s="2">
         <v>45571</v>
@@ -5559,9 +5553,9 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="2">
         <v>45582</v>
@@ -5570,9 +5564,9 @@
         <v>0.51500000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" s="2">
         <v>45594</v>
@@ -5581,9 +5575,9 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" s="2">
         <v>45609</v>
@@ -5592,9 +5586,9 @@
         <v>0.11749999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="2">
         <v>45443</v>
@@ -5603,9 +5597,9 @@
         <v>0.27750000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" s="2">
         <v>45460</v>
@@ -5614,9 +5608,9 @@
         <v>0.35749999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" s="2">
         <v>45474</v>
@@ -5625,9 +5619,9 @@
         <v>0.48749999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" s="2">
         <v>45487</v>
@@ -5636,9 +5630,9 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" s="2">
         <v>45502</v>
@@ -5647,9 +5641,9 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" s="2">
         <v>45513</v>
@@ -5658,9 +5652,9 @@
         <v>0.58499999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="2">
         <v>45526</v>
@@ -5669,9 +5663,9 @@
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" s="2">
         <v>45548</v>
@@ -5680,9 +5674,9 @@
         <v>0.80249999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="2">
         <v>45559</v>
@@ -5691,9 +5685,9 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" s="2">
         <v>45571</v>
@@ -5702,9 +5696,9 @@
         <v>0.72249999999999992</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" s="2">
         <v>45582</v>
@@ -5713,9 +5707,9 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" s="2">
         <v>45594</v>
@@ -5724,9 +5718,9 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="2">
         <v>45609</v>
@@ -5735,9 +5729,9 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B54" s="2">
         <v>45443</v>
@@ -5746,9 +5740,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B55" s="2">
         <v>45460</v>
@@ -5757,9 +5751,9 @@
         <v>0.17249999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B56" s="2">
         <v>45474</v>
@@ -5768,9 +5762,9 @@
         <v>0.25750000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B57" s="2">
         <v>45487</v>
@@ -5779,9 +5773,9 @@
         <v>0.3725</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B58" s="2">
         <v>45502</v>
@@ -5790,9 +5784,9 @@
         <v>0.495</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B59" s="2">
         <v>45513</v>
@@ -5801,9 +5795,9 @@
         <v>0.59499999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B60" s="2">
         <v>45526</v>
@@ -5812,9 +5806,9 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B61" s="2">
         <v>45548</v>
@@ -5823,9 +5817,9 @@
         <v>0.83499999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" s="2">
         <v>45559</v>
@@ -5834,9 +5828,9 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B63" s="2">
         <v>45571</v>
@@ -5845,9 +5839,9 @@
         <v>0.745</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B64" s="2">
         <v>45582</v>
@@ -5856,9 +5850,9 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" s="2">
         <v>45594</v>
@@ -5867,9 +5861,9 @@
         <v>0.40250000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B66" s="2">
         <v>45609</v>
@@ -5878,9 +5872,9 @@
         <v>0.1275</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" s="2">
         <v>45443</v>
@@ -5889,9 +5883,9 @@
         <v>0.17249999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B68" s="2">
         <v>45460</v>
@@ -5900,9 +5894,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B69" s="2">
         <v>45474</v>
@@ -5911,9 +5905,9 @@
         <v>0.23749999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B70" s="2">
         <v>45487</v>
@@ -5922,9 +5916,9 @@
         <v>0.33250000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B71" s="2">
         <v>45502</v>
@@ -5933,9 +5927,9 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B72" s="2">
         <v>45513</v>
@@ -5944,9 +5938,9 @@
         <v>0.54500000000000004</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B73" s="2">
         <v>45526</v>
@@ -5955,9 +5949,9 @@
         <v>0.64250000000000007</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B74" s="2">
         <v>45548</v>
@@ -5966,9 +5960,9 @@
         <v>0.7975000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B75" s="2">
         <v>45559</v>
@@ -5977,9 +5971,9 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B76" s="2">
         <v>45571</v>
@@ -5988,9 +5982,9 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B77" s="2">
         <v>45582</v>
@@ -5999,9 +5993,9 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B78" s="2">
         <v>45594</v>
@@ -6010,9 +6004,9 @@
         <v>0.38750000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B79" s="2">
         <v>45609</v>
@@ -6021,9 +6015,9 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B80" s="2">
         <v>45443</v>
@@ -6032,9 +6026,9 @@
         <v>0.16750000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B81" s="2">
         <v>45460</v>
@@ -6043,9 +6037,9 @@
         <v>0.1575</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B82" s="2">
         <v>45474</v>
@@ -6054,9 +6048,9 @@
         <v>0.215</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B83" s="2">
         <v>45487</v>
@@ -6065,9 +6059,9 @@
         <v>0.3175</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B84" s="2">
         <v>45502</v>
@@ -6076,9 +6070,9 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B85" s="2">
         <v>45513</v>
@@ -6087,9 +6081,9 @@
         <v>0.505</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B86" s="2">
         <v>45526</v>
@@ -6098,9 +6092,9 @@
         <v>0.61499999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B87" s="2">
         <v>45548</v>
@@ -6109,9 +6103,9 @@
         <v>0.77750000000000008</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B88" s="2">
         <v>45559</v>
@@ -6120,9 +6114,9 @@
         <v>0.74750000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B89" s="2">
         <v>45571</v>
@@ -6131,9 +6125,9 @@
         <v>0.70250000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B90" s="2">
         <v>45582</v>
@@ -6142,9 +6136,9 @@
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B91" s="2">
         <v>45594</v>
@@ -6153,9 +6147,9 @@
         <v>0.40749999999999997</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B92" s="2">
         <v>45609</v>
@@ -6164,9 +6158,9 @@
         <v>0.1225</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B93" s="2">
         <v>45443</v>
@@ -6175,9 +6169,9 @@
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B94" s="2">
         <v>45460</v>
@@ -6186,9 +6180,9 @@
         <v>0.1925</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B95" s="2">
         <v>45474</v>
@@ -6197,9 +6191,9 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B96" s="2">
         <v>45487</v>
@@ -6208,9 +6202,9 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B97" s="2">
         <v>45502</v>
@@ -6219,9 +6213,9 @@
         <v>0.56500000000000006</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B98" s="2">
         <v>45513</v>
@@ -6230,9 +6224,9 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B99" s="2">
         <v>45526</v>
@@ -6241,9 +6235,9 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B100" s="2">
         <v>45548</v>
@@ -6252,9 +6246,9 @@
         <v>0.83250000000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B101" s="2">
         <v>45559</v>
@@ -6263,9 +6257,9 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B102" s="2">
         <v>45571</v>
@@ -6274,9 +6268,9 @@
         <v>0.755</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B103" s="2">
         <v>45582</v>
@@ -6285,9 +6279,9 @@
         <v>0.59750000000000003</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B104" s="2">
         <v>45594</v>
@@ -6296,9 +6290,9 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B105" s="2">
         <v>45609</v>
@@ -6307,9 +6301,9 @@
         <v>0.1275</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B106" s="2">
         <v>45436</v>
@@ -6318,9 +6312,9 @@
         <v>3.8250000000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B107" s="2">
         <v>45446</v>
@@ -6329,9 +6323,9 @@
         <v>4.8916666666666666</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B108" s="2">
         <v>45457</v>
@@ -6340,9 +6334,9 @@
         <v>6.0583333333333327</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B109" s="2">
         <v>45468</v>
@@ -6351,9 +6345,9 @@
         <v>6.5833333333333339</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B110" s="2">
         <v>45483</v>
@@ -6362,9 +6356,9 @@
         <v>7.4666666666666668</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B111" s="2">
         <v>45495</v>
@@ -6373,9 +6367,9 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B112" s="2">
         <v>45513</v>
@@ -6384,9 +6378,9 @@
         <v>9.4749999999999996</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B113" s="2">
         <v>45522</v>
@@ -6395,9 +6389,9 @@
         <v>10.258333333333329</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B114" s="2">
         <v>45532</v>
@@ -6406,9 +6400,9 @@
         <v>11.56666666666667</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B115" s="2">
         <v>45550</v>
@@ -6417,9 +6411,9 @@
         <v>13.33333333333333</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B116" s="2">
         <v>45559</v>
@@ -6428,9 +6422,9 @@
         <v>13.875</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B117" s="2">
         <v>45436</v>
@@ -6439,9 +6433,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B118" s="2">
         <v>45446</v>
@@ -6450,9 +6444,9 @@
         <v>4.8999999999999986</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B119" s="2">
         <v>45457</v>
@@ -6461,9 +6455,9 @@
         <v>6.2833333333333332</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B120" s="2">
         <v>45468</v>
@@ -6472,9 +6466,9 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B121" s="2">
         <v>45483</v>
@@ -6483,9 +6477,9 @@
         <v>7.6750000000000007</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B122" s="2">
         <v>45495</v>
@@ -6494,9 +6488,9 @@
         <v>8.4916666666666671</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B123" s="2">
         <v>45513</v>
@@ -6505,9 +6499,9 @@
         <v>9.8833333333333329</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B124" s="2">
         <v>45522</v>
@@ -6516,9 +6510,9 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B125" s="2">
         <v>45532</v>
@@ -6527,9 +6521,9 @@
         <v>11.83333333333333</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B126" s="2">
         <v>45550</v>
@@ -6538,9 +6532,9 @@
         <v>12.58333333333333</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B127" s="2">
         <v>45436</v>
@@ -6549,9 +6543,9 @@
         <v>4.1916666666666664</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B128" s="2">
         <v>45446</v>
@@ -6560,9 +6554,9 @@
         <v>5.1916666666666664</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B129" s="2">
         <v>45457</v>
@@ -6571,9 +6565,9 @@
         <v>6.208333333333333</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B130" s="2">
         <v>45468</v>
@@ -6582,9 +6576,9 @@
         <v>6.833333333333333</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B131" s="2">
         <v>45483</v>
@@ -6593,9 +6587,9 @@
         <v>7.7583333333333337</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B132" s="2">
         <v>45495</v>
@@ -6604,9 +6598,9 @@
         <v>8.5666666666666664</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B133" s="2">
         <v>45513</v>
@@ -6615,9 +6609,9 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B134" s="2">
         <v>45522</v>
@@ -6626,9 +6620,9 @@
         <v>10.95</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B135" s="2">
         <v>45532</v>
@@ -6637,9 +6631,9 @@
         <v>11.78333333333333</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B136" s="2">
         <v>45550</v>
@@ -6648,9 +6642,9 @@
         <v>12.16666666666667</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B137" s="2">
         <v>45436</v>
@@ -6659,9 +6653,9 @@
         <v>4.1916666666666664</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B138" s="2">
         <v>45446</v>
@@ -6670,9 +6664,9 @@
         <v>5.2333333333333334</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B139" s="2">
         <v>45457</v>
@@ -6681,9 +6675,9 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B140" s="2">
         <v>45468</v>
@@ -6692,9 +6686,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B141" s="2">
         <v>45483</v>
@@ -6703,9 +6697,9 @@
         <v>7.9666666666666668</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B142" s="2">
         <v>45495</v>
@@ -6714,9 +6708,9 @@
         <v>8.8333333333333339</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B143" s="2">
         <v>45513</v>
@@ -6725,9 +6719,9 @@
         <v>10.275</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B144" s="2">
         <v>45522</v>
@@ -6736,9 +6730,9 @@
         <v>11.258333333333329</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B145" s="2">
         <v>45532</v>
@@ -6747,9 +6741,9 @@
         <v>12.483333333333331</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B146" s="2">
         <v>45550</v>
@@ -6758,9 +6752,9 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B147" s="2">
         <v>45467</v>
@@ -6769,9 +6763,9 @@
         <v>3.066666666666666</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B148" s="2">
         <v>45477</v>
@@ -6780,9 +6774,9 @@
         <v>3.8083333333333331</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B149" s="2">
         <v>45488</v>
@@ -6791,9 +6785,9 @@
         <v>4.6500000000000004</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B150" s="2">
         <v>45499</v>
@@ -6802,9 +6796,9 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B151" s="2">
         <v>45513</v>
@@ -6813,9 +6807,9 @@
         <v>6.65</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B152" s="2">
         <v>45523</v>
@@ -6824,9 +6818,9 @@
         <v>7.6916666666666664</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B153" s="2">
         <v>45535</v>
@@ -6835,9 +6829,9 @@
         <v>9.0083333333333329</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B154" s="2">
         <v>45550</v>
@@ -6846,9 +6840,9 @@
         <v>10.08333333333333</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B155" s="2">
         <v>45467</v>
@@ -6857,9 +6851,9 @@
         <v>3.041666666666667</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B156" s="2">
         <v>45477</v>
@@ -6868,9 +6862,9 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B157" s="2">
         <v>45488</v>
@@ -6879,9 +6873,9 @@
         <v>4.8416666666666668</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B158" s="2">
         <v>45499</v>
@@ -6890,9 +6884,9 @@
         <v>5.8249999999999993</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B159" s="2">
         <v>45513</v>
@@ -6901,9 +6895,9 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B160" s="2">
         <v>45523</v>
@@ -6912,9 +6906,9 @@
         <v>8.1083333333333343</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B161" s="2">
         <v>45535</v>
@@ -6923,9 +6917,9 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B162" s="2">
         <v>45550</v>
@@ -6934,9 +6928,9 @@
         <v>10.608333333333331</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B163" s="2">
         <v>45559</v>
@@ -6945,9 +6939,9 @@
         <v>10.66666666666667</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B164" s="2">
         <v>45467</v>
@@ -6956,9 +6950,9 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B165" s="2">
         <v>45477</v>
@@ -6967,9 +6961,9 @@
         <v>3.9249999999999998</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B166" s="2">
         <v>45488</v>
@@ -6978,9 +6972,9 @@
         <v>4.9583333333333339</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B167" s="2">
         <v>45499</v>
@@ -6989,9 +6983,9 @@
         <v>6.0083333333333329</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B168" s="2">
         <v>45513</v>
@@ -7000,9 +6994,9 @@
         <v>7.1083333333333334</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B169" s="2">
         <v>45523</v>
@@ -7011,9 +7005,9 @@
         <v>8.2249999999999996</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B170" s="2">
         <v>45535</v>
@@ -7022,9 +7016,9 @@
         <v>9.8249999999999993</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B171" s="2">
         <v>45550</v>
@@ -7033,9 +7027,9 @@
         <v>11.266666666666669</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B172" s="2">
         <v>45559</v>
@@ -7044,9 +7038,9 @@
         <v>11.66666666666667</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B173" s="2">
         <v>45467</v>
@@ -7055,9 +7049,9 @@
         <v>3.1583333333333332</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B174" s="2">
         <v>45477</v>
@@ -7066,9 +7060,9 @@
         <v>4.2583333333333329</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B175" s="2">
         <v>45488</v>
@@ -7077,9 +7071,9 @@
         <v>5.3250000000000002</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B176" s="2">
         <v>45499</v>
@@ -7088,9 +7082,9 @@
         <v>6.375</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B177" s="2">
         <v>45513</v>
@@ -7099,9 +7093,9 @@
         <v>7.4833333333333334</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B178" s="2">
         <v>45523</v>
@@ -7110,9 +7104,9 @@
         <v>8.5166666666666657</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B179" s="2">
         <v>45535</v>
@@ -7121,9 +7115,9 @@
         <v>9.875</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B180" s="2">
         <v>45550</v>
@@ -7132,9 +7126,9 @@
         <v>11.20833333333333</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B181" s="2">
         <v>45559</v>
@@ -7143,9 +7137,9 @@
         <v>11.58333333333333</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B182" s="2">
         <v>45409</v>
@@ -7154,9 +7148,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B183" s="2">
         <v>45410</v>
@@ -7165,9 +7159,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B184" s="2">
         <v>45409</v>
@@ -7176,9 +7170,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B185" s="2">
         <v>45411</v>
@@ -7187,9 +7181,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B186" s="2">
         <v>45439</v>
@@ -7198,9 +7192,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B187" s="2">
         <v>45439</v>
@@ -7209,9 +7203,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B188" s="2">
         <v>45439</v>
@@ -7220,9 +7214,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B189" s="2">
         <v>45438</v>
@@ -7231,9 +7225,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B190" s="2">
         <v>45558</v>
@@ -7242,9 +7236,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B191" s="2">
         <v>45543</v>
@@ -7253,9 +7247,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B192" s="2">
         <v>45538</v>
@@ -7264,9 +7258,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B193" s="2">
         <v>45541</v>
@@ -7275,9 +7269,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B194" s="2">
         <v>45547</v>
@@ -7286,9 +7280,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B195" s="2">
         <v>45549</v>
@@ -7297,9 +7291,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B196" s="2">
         <v>45551</v>
@@ -7308,9 +7302,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B197" s="2">
         <v>45551</v>
@@ -7319,9 +7313,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B198" s="2">
         <v>45574</v>
@@ -7330,9 +7324,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B199" s="2">
         <v>45566</v>
@@ -7341,9 +7335,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B200" s="2">
         <v>45560</v>
@@ -7352,9 +7346,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B201" s="2">
         <v>45561</v>
@@ -7363,9 +7357,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B202" s="2">
         <v>45569</v>
@@ -7374,9 +7368,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B203" s="2">
         <v>45568</v>
@@ -7385,9 +7379,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B204" s="2">
         <v>45570</v>
@@ -7396,9 +7390,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B205" s="2">
         <v>45572</v>
@@ -7407,9 +7401,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B206" s="2">
         <v>45559</v>
@@ -7442,9 +7436,9 @@
         <v>60.888654410591528</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B207" s="2">
         <v>45544</v>
@@ -7477,9 +7471,9 @@
         <v>35.839836166008233</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B208" s="2">
         <v>45541</v>
@@ -7512,9 +7506,9 @@
         <v>62.748999492773287</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B209" s="2">
         <v>45541</v>
@@ -7547,9 +7541,9 @@
         <v>39.273120931761547</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B210" s="2">
         <v>45548</v>
@@ -7582,9 +7576,9 @@
         <v>32.451262390143462</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B211" s="2">
         <v>45551</v>
@@ -7617,9 +7611,9 @@
         <v>48.686760023628644</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B212" s="2">
         <v>45551</v>
@@ -7652,9 +7646,9 @@
         <v>29.8698997468404</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B213" s="2">
         <v>45551</v>
@@ -7687,9 +7681,9 @@
         <v>18.150858440559141</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B214" s="2">
         <v>45573</v>
@@ -7719,9 +7713,9 @@
         <v>176.15308909985779</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B215" s="2">
         <v>45566</v>
@@ -7751,9 +7745,9 @@
         <v>187.98152286098309</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B216" s="2">
         <v>45560</v>
@@ -7783,9 +7777,9 @@
         <v>233.7931264152482</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B217" s="2">
         <v>45561</v>
@@ -7815,9 +7809,9 @@
         <v>182.822191121505</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B218" s="2">
         <v>45568</v>
@@ -7847,9 +7841,9 @@
         <v>159.45722446674071</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B219" s="2">
         <v>45568</v>
@@ -7879,9 +7873,9 @@
         <v>172.85553289550279</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B220" s="2">
         <v>45573</v>
@@ -7911,9 +7905,9 @@
         <v>177.83588521473811</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B221" s="2">
         <v>45573</v>
@@ -7943,9 +7937,9 @@
         <v>161.63552037236391</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B222" s="2">
         <v>45610</v>
@@ -7975,12 +7969,12 @@
         <v>15163.62934093144</v>
       </c>
       <c r="Q222" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B223" s="2">
         <v>45610</v>
@@ -8010,12 +8004,12 @@
         <v>11717.491854334879</v>
       </c>
       <c r="Q223" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B224" s="2">
         <v>45610</v>
@@ -8045,12 +8039,12 @@
         <v>17964.896618129951</v>
       </c>
       <c r="Q224" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B225" s="2">
         <v>45610</v>
@@ -8080,12 +8074,12 @@
         <v>15964.97578041526</v>
       </c>
       <c r="Q225" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B226" s="2">
         <v>45610</v>
@@ -8115,12 +8109,12 @@
         <v>15332.992480958441</v>
       </c>
       <c r="Q226" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B227" s="2">
         <v>45610</v>
@@ -8150,12 +8144,12 @@
         <v>13478.15972223027</v>
       </c>
       <c r="Q227" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B228" s="2">
         <v>45610</v>
@@ -8185,12 +8179,12 @@
         <v>15257.677335938009</v>
       </c>
       <c r="Q228" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B229" s="2">
         <v>45610</v>
@@ -8220,7 +8214,7 @@
         <v>9738.7459024403233</v>
       </c>
       <c r="Q229" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -8232,65 +8226,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10428EF5-B0F7-41D7-9FD7-1C8CB347A925}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F3">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="7" t="str">
         <f>VLOOKUP(G11,$F$1:$G$4,2,FALSE)</f>
@@ -8305,7 +8299,7 @@
         <v>[Wheat].Phenology.Flowering.DateToProgress</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -8317,7 +8311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="str">
         <f>F12</f>
         <v>DookieEVA2024SowApril_BigRed</v>
@@ -8335,7 +8329,7 @@
         <v>45574</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G12" s="5">
         <v>45409</v>
@@ -8347,7 +8341,7 @@
         <v>45574</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="str">
         <f t="shared" ref="A13:A19" si="1">F13</f>
         <v>DookieEVA2024SowApril_Illabo</v>
@@ -8365,7 +8359,7 @@
         <v>45566</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="5">
         <v>45410</v>
@@ -8377,7 +8371,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="str">
         <f t="shared" si="1"/>
         <v>DookieEVA2024SowApril_UOM001_3_47</v>
@@ -8395,7 +8389,7 @@
         <v>45560</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="5">
         <v>45409</v>
@@ -8407,7 +8401,7 @@
         <v>45560</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="str">
         <f t="shared" si="1"/>
         <v>DookieEVA2024SowApril_UOM001_9_1</v>
@@ -8425,7 +8419,7 @@
         <v>45561</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="5">
         <v>45411</v>
@@ -8437,7 +8431,7 @@
         <v>45561</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f t="shared" si="1"/>
         <v>DookieEVA2024SowMay_Sunmaster</v>
@@ -8455,7 +8449,7 @@
         <v>45569</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="5">
         <v>45439</v>
@@ -8467,7 +8461,7 @@
         <v>45569</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f t="shared" si="1"/>
         <v>DookieEVA2024SowMay_UOM001_3_47</v>
@@ -8485,7 +8479,7 @@
         <v>45568</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17" s="5">
         <v>45439</v>
@@ -8497,7 +8491,7 @@
         <v>45568</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="str">
         <f t="shared" si="1"/>
         <v>DookieEVA2024SowMay_UOM001_9_1</v>
@@ -8515,7 +8509,7 @@
         <v>45570</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="5">
         <v>45439</v>
@@ -8527,7 +8521,7 @@
         <v>45570</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="str">
         <f t="shared" si="1"/>
         <v>DookieEVA2024SowMay_Zanzibar</v>
@@ -8545,7 +8539,7 @@
         <v>45572</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="5">
         <v>45438</v>

</xml_diff>